<commit_message>
added mixture ratio and Isp analysis docs
</commit_message>
<xml_diff>
--- a/Nozzle-CC/C-Engine.xlsx
+++ b/Nozzle-CC/C-Engine.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nyameaama/Documents/A-OneSpace/Converse-Engine/Nozzle-CC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F76779D3-825E-BC49-A93D-3A7871DB7ABD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AF1E794-E423-8040-ABE3-FC8A1420A5C0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14520" yWindow="0" windowWidth="14280" windowHeight="18000" tabRatio="920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14520" yWindow="500" windowWidth="14280" windowHeight="16260" tabRatio="920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VesselCharacteristics" sheetId="14" r:id="rId1"/>
@@ -3129,7 +3129,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -3138,12 +3138,21 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-This is a measure of the loss in flow efficiency due to an imperfect design. 1 would be perfect. Note it is possible to calculate this as a function of the reynolds number, however, for rough approximations, the flow coefficient may be assumed to be between 0.60 and 0.75. For a first approximation, a flow coefficient of 0.62 can be used as this approximates to fully developed flow.</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This is a measure of the loss in flow efficiency due to an imperfect design. 1 would be perfect. Note it is possible to calculate this as a function of the reynolds number, however, for rough approximations, the flow coefficient may be assumed to be between 0.60 and 0.75. For a first approximation, a flow coefficient of 0.62 can be used as this approximates to fully developed flow.</t>
         </r>
       </text>
     </comment>
@@ -47107,8 +47116,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:IV100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="116" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D59" sqref="D59"/>
+    <sheetView tabSelected="1" zoomScale="116" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>